<commit_message>
Worked on sending messages with files
</commit_message>
<xml_diff>
--- a/test_resourses/test_dir.xlsx
+++ b/test_resourses/test_dir.xlsx
@@ -20,9 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teléfono</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAIL</t>
+  </si>
   <si>
     <t xml:space="preserve">Rodrigo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
   </si>
   <si>
     <t xml:space="preserve">Rubén</t>
@@ -46,6 +61,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -105,8 +121,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -233,44 +257,89 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.66"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="str">
+        <f aca="false"> _xlfn.CONCAT(B2,C2)</f>
+        <v>Rodrigo5545125300</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>5545125300</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="str">
+        <f aca="false"> _xlfn.CONCAT(B3,C3)</f>
+        <v>Rubén5522654896</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>5522654896</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="n">
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="str">
+        <f aca="false"> _xlfn.CONCAT(B4,C4)</f>
+        <v>Lilia5510721906</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>5510721906</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="n">
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="str">
+        <f aca="false"> _xlfn.CONCAT(B5,C5)</f>
+        <v>Diego5526547119</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>5526547119</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on sending files using selenium to multiple contacts. To work on refactoring
</commit_message>
<xml_diff>
--- a/test_resourses/test_dir.xlsx
+++ b/test_resourses/test_dir.xlsx
@@ -22,13 +22,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teléfono</t>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TELEFONO</t>
   </si>
   <si>
     <t xml:space="preserve">EMAIL</t>
@@ -126,11 +126,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -260,37 +260,37 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="str">
-        <f aca="false"> _xlfn.CONCAT(B2,C2)</f>
+      <c r="A2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(B2,C2)</f>
         <v>Rodrigo5545125300</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="2" t="n">
         <v>5545125300</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -298,14 +298,14 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="str">
-        <f aca="false"> _xlfn.CONCAT(B3,C3)</f>
+      <c r="A3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(B3,C3)</f>
         <v>Rubén5522654896</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="n">
         <v>5522654896</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -313,14 +313,14 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="str">
-        <f aca="false"> _xlfn.CONCAT(B4,C4)</f>
+      <c r="A4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(B4,C4)</f>
         <v>Lilia5510721906</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="2" t="n">
         <v>5510721906</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -328,14 +328,14 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="str">
-        <f aca="false"> _xlfn.CONCAT(B5,C5)</f>
+      <c r="A5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT(B5,C5)</f>
         <v>Diego5526547119</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="2" t="n">
         <v>5526547119</v>
       </c>
       <c r="D5" s="2" t="s">

</xml_diff>